<commit_message>
i should have used a for loop
</commit_message>
<xml_diff>
--- a/sensitivity analysis/outputs/S6/S6_start_immunity.xlsx
+++ b/sensitivity analysis/outputs/S6/S6_start_immunity.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,32 +377,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>overall_imm_death_lower</t>
+          <t>immunity_all</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>infection_and_vaccination_death_pct_lower</t>
+          <t>immunity_by_infection</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>infection_only_death_pct_lower</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>vaccination_only_death_pct_lower</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>scenario</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>excess</t>
+          <t>immunity_by_vaccination</t>
         </is>
       </c>
     </row>
@@ -422,18 +407,7 @@
         <v>27.69389020031914</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>17.11959580917898</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H2">
-        <v>-17.11959580917898</v>
+        <v>44.81348600949812</v>
       </c>
     </row>
     <row r="3">
@@ -449,21 +423,10 @@
         <v>34.72731820352276</v>
       </c>
       <c r="D3">
+        <v>34.72731820352275</v>
+      </c>
+      <c r="E3">
         <v>30.0654685149135</v>
-      </c>
-      <c r="E3">
-        <v>4.66184968860925</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H3">
-        <v>4.66184968860925</v>
       </c>
     </row>
     <row r="4">
@@ -482,18 +445,7 @@
         <v>8.385509838998209</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>42.39442257302976</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H4">
-        <v>-42.39442257302976</v>
+        <v>50.77993241202797</v>
       </c>
     </row>
     <row r="5">
@@ -509,21 +461,10 @@
         <v>34.59715932609676</v>
       </c>
       <c r="D5">
+        <v>34.59715932609676</v>
+      </c>
+      <c r="E5">
         <v>27.92224978552357</v>
-      </c>
-      <c r="E5">
-        <v>6.674909540573188</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H5">
-        <v>6.674909540573188</v>
       </c>
     </row>
     <row r="6">
@@ -542,18 +483,7 @@
         <v>25.77179363093073</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>15.02474103082425</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H6">
-        <v>-15.02474103082425</v>
+        <v>40.79653466175498</v>
       </c>
     </row>
     <row r="7">
@@ -572,18 +502,7 @@
         <v>25.48576751707107</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>20.6116403294074</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H7">
-        <v>-20.6116403294074</v>
+        <v>46.09740784647846</v>
       </c>
     </row>
     <row r="8">
@@ -602,18 +521,7 @@
         <v>34.89980169084647</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>8.273549837432327</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H8">
-        <v>-8.273549837432327</v>
+        <v>43.17335152827879</v>
       </c>
     </row>
     <row r="9">
@@ -632,18 +540,7 @@
         <v>36.51663094387552</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>4.744309677262969</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H9">
-        <v>-4.744309677262969</v>
+        <v>41.26094062113849</v>
       </c>
     </row>
     <row r="10">
@@ -662,18 +559,7 @@
         <v>25.78915980298924</v>
       </c>
       <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>7.272555716349105</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H10">
-        <v>-7.272555716349105</v>
+        <v>33.06171551933835</v>
       </c>
     </row>
     <row r="11">
@@ -692,18 +578,7 @@
         <v>18.20733603914577</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>30.86015280564254</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H11">
-        <v>-30.86015280564254</v>
+        <v>49.06748884478831</v>
       </c>
     </row>
     <row r="12">
@@ -722,18 +597,7 @@
         <v>19.40399782244024</v>
       </c>
       <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>27.38364955714526</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H12">
-        <v>-27.38364955714526</v>
+        <v>46.7876473795855</v>
       </c>
     </row>
     <row r="13">
@@ -752,18 +616,7 @@
         <v>27.70215734825373</v>
       </c>
       <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>3.412066041434335</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H13">
-        <v>-3.412066041434335</v>
+        <v>31.11422338968807</v>
       </c>
     </row>
     <row r="14">
@@ -782,18 +635,7 @@
         <v>19.43413893175528</v>
       </c>
       <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>11.34758563239342</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H14">
-        <v>-11.34758563239342</v>
+        <v>30.7817245641487</v>
       </c>
     </row>
     <row r="15">
@@ -812,18 +654,7 @@
         <v>31.37646877571649</v>
       </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0.8096393480855701</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H15">
-        <v>-0.8096393480855701</v>
+        <v>32.18610812380206</v>
       </c>
     </row>
     <row r="16">
@@ -842,18 +673,7 @@
         <v>11.66495337663947</v>
       </c>
       <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>20.40693956666923</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H16">
-        <v>-20.40693956666923</v>
+        <v>32.07189294330869</v>
       </c>
     </row>
     <row r="17">
@@ -872,18 +692,7 @@
         <v>12.4734104754374</v>
       </c>
       <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>28.158852001571</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H17">
-        <v>-28.158852001571</v>
+        <v>40.6322624770084</v>
       </c>
     </row>
     <row r="18">
@@ -902,18 +711,7 @@
         <v>21.70286070832712</v>
       </c>
       <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>16.29091906663612</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H18">
-        <v>-16.29091906663612</v>
+        <v>37.99377977496324</v>
       </c>
     </row>
     <row r="19">
@@ -932,18 +730,7 @@
         <v>30.16151049625446</v>
       </c>
       <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>3.610315275238249</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H19">
-        <v>-3.610315275238249</v>
+        <v>33.77182577149271</v>
       </c>
     </row>
     <row r="20">
@@ -962,18 +749,7 @@
         <v>19.40922628354292</v>
       </c>
       <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>30.04084163678851</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H20">
-        <v>-30.04084163678851</v>
+        <v>49.45006792033143</v>
       </c>
     </row>
     <row r="21">
@@ -992,18 +768,7 @@
         <v>21.45232221387965</v>
       </c>
       <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>9.336265335512893</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H21">
-        <v>-9.336265335512893</v>
+        <v>30.78858754939254</v>
       </c>
     </row>
     <row r="22">
@@ -1022,18 +787,7 @@
         <v>45.83626630870725</v>
       </c>
       <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>1.09224718742824</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H22">
-        <v>-1.09224718742824</v>
+        <v>46.92851349613549</v>
       </c>
     </row>
     <row r="23">
@@ -1052,18 +806,7 @@
         <v>26.7045214971398</v>
       </c>
       <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>8.204606698461879</v>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H23">
-        <v>-8.204606698461879</v>
+        <v>34.90912819560168</v>
       </c>
     </row>
     <row r="24">
@@ -1079,21 +822,10 @@
         <v>36.53138457110415</v>
       </c>
       <c r="D24">
+        <v>36.53138457110415</v>
+      </c>
+      <c r="E24">
         <v>34.63768001177167</v>
-      </c>
-      <c r="E24">
-        <v>1.893704559332476</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H24">
-        <v>1.893704559332476</v>
       </c>
     </row>
     <row r="25">
@@ -1109,21 +841,10 @@
         <v>41.98198890358411</v>
       </c>
       <c r="D25">
+        <v>41.98198890358411</v>
+      </c>
+      <c r="E25">
         <v>28.70112580140914</v>
-      </c>
-      <c r="E25">
-        <v>13.28086310217496</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H25">
-        <v>13.28086310217496</v>
       </c>
     </row>
     <row r="26">
@@ -1142,18 +863,7 @@
         <v>19.21369456079821</v>
       </c>
       <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>14.00334805858523</v>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H26">
-        <v>-14.00334805858523</v>
+        <v>33.21704261938344</v>
       </c>
     </row>
     <row r="27">
@@ -1172,18 +882,7 @@
         <v>14.83640780524465</v>
       </c>
       <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>6.371247822341701</v>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H27">
-        <v>-6.371247822341701</v>
+        <v>21.20765562758635</v>
       </c>
     </row>
     <row r="28">
@@ -1202,18 +901,7 @@
         <v>9.920663867483272</v>
       </c>
       <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>25.91987186251877</v>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H28">
-        <v>-25.91987186251877</v>
+        <v>35.84053573000205</v>
       </c>
     </row>
     <row r="29">
@@ -1232,18 +920,7 @@
         <v>4.672043764308133</v>
       </c>
       <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>59.16374256293692</v>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H29">
-        <v>-59.16374256293692</v>
+        <v>63.83578632724505</v>
       </c>
     </row>
     <row r="30">
@@ -1262,18 +939,7 @@
         <v>18.60505787800943</v>
       </c>
       <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>12.40053025294186</v>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H30">
-        <v>-12.40053025294186</v>
+        <v>31.00558813095128</v>
       </c>
     </row>
     <row r="31">
@@ -1292,18 +958,7 @@
         <v>14.92697614050289</v>
       </c>
       <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>24.11184711931735</v>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H31">
-        <v>-24.11184711931735</v>
+        <v>39.03882325982025</v>
       </c>
     </row>
     <row r="32">
@@ -1319,21 +974,10 @@
         <v>37.83080758338105</v>
       </c>
       <c r="D32">
+        <v>37.83080758338104</v>
+      </c>
+      <c r="E32">
         <v>28.58253284614246</v>
-      </c>
-      <c r="E32">
-        <v>9.248274737238591</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H32">
-        <v>9.248274737238591</v>
       </c>
     </row>
     <row r="33">
@@ -1352,18 +996,7 @@
         <v>11.79075407545688</v>
       </c>
       <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33">
-        <v>34.67756030680075</v>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H33">
-        <v>-34.67756030680075</v>
+        <v>46.46831438225763</v>
       </c>
     </row>
     <row r="34">
@@ -1379,21 +1012,10 @@
         <v>33.31268336586677</v>
       </c>
       <c r="D34">
+        <v>33.31268336586677</v>
+      </c>
+      <c r="E34">
         <v>32.06924299347569</v>
-      </c>
-      <c r="E34">
-        <v>1.243440372391083</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H34">
-        <v>1.243440372391083</v>
       </c>
     </row>
     <row r="35">
@@ -1412,18 +1034,7 @@
         <v>17.59085275656659</v>
       </c>
       <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>23.48721904716486</v>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H35">
-        <v>-23.48721904716486</v>
+        <v>41.07807180373145</v>
       </c>
     </row>
     <row r="36">
@@ -1442,18 +1053,7 @@
         <v>12.75057783300452</v>
       </c>
       <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>19.37788694157747</v>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H36">
-        <v>-19.37788694157747</v>
+        <v>32.12846477458199</v>
       </c>
     </row>
     <row r="37">
@@ -1472,18 +1072,7 @@
         <v>31.15217803890725</v>
       </c>
       <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0.6450665699890809</v>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H37">
-        <v>-0.6450665699890809</v>
+        <v>31.79724460889633</v>
       </c>
     </row>
     <row r="38">
@@ -1502,18 +1091,7 @@
         <v>18.65124830140416</v>
       </c>
       <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>13.32703931931475</v>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H38">
-        <v>-13.32703931931475</v>
+        <v>31.97828762071891</v>
       </c>
     </row>
     <row r="39">
@@ -1529,21 +1107,10 @@
         <v>36.16080710921468</v>
       </c>
       <c r="D39">
+        <v>36.16080710921468</v>
+      </c>
+      <c r="E39">
         <v>32.0937866595111</v>
-      </c>
-      <c r="E39">
-        <v>4.067020449703575</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H39">
-        <v>4.067020449703575</v>
       </c>
     </row>
     <row r="40">
@@ -1562,18 +1129,7 @@
         <v>22.56036843415483</v>
       </c>
       <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>21.33128600619761</v>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H40">
-        <v>-21.33128600619761</v>
+        <v>43.89165444035244</v>
       </c>
     </row>
     <row r="41">
@@ -1592,18 +1148,7 @@
         <v>35.10966283751906</v>
       </c>
       <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>1.850816862533334</v>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H41">
-        <v>-1.850816862533334</v>
+        <v>36.9604797000524</v>
       </c>
     </row>
     <row r="42">
@@ -1622,18 +1167,7 @@
         <v>21.30486001453744</v>
       </c>
       <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>20.05145954085538</v>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H42">
-        <v>-20.05145954085538</v>
+        <v>41.35631955539282</v>
       </c>
     </row>
     <row r="43">
@@ -1649,21 +1183,10 @@
         <v>34.86257832809894</v>
       </c>
       <c r="D43">
+        <v>34.86257832809895</v>
+      </c>
+      <c r="E43">
         <v>33.9806992108897</v>
-      </c>
-      <c r="E43">
-        <v>0.8818791172092418</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H43">
-        <v>0.8818791172092418</v>
       </c>
     </row>
     <row r="44">
@@ -1682,18 +1205,7 @@
         <v>21.16674100224519</v>
       </c>
       <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>5.434890041390688</v>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H44">
-        <v>-5.434890041390688</v>
+        <v>26.60163104363588</v>
       </c>
     </row>
     <row r="45">
@@ -1712,18 +1224,7 @@
         <v>32.25444727090838</v>
       </c>
       <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>15.48878968246249</v>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H45">
-        <v>-15.48878968246249</v>
+        <v>47.74323695337088</v>
       </c>
     </row>
     <row r="46">
@@ -1742,18 +1243,7 @@
         <v>24.23237914435604</v>
       </c>
       <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>23.74145347561217</v>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H46">
-        <v>-23.74145347561217</v>
+        <v>47.97383261996821</v>
       </c>
     </row>
     <row r="47">
@@ -1769,21 +1259,10 @@
         <v>41.64584374479427</v>
       </c>
       <c r="D47">
+        <v>41.64584374479427</v>
+      </c>
+      <c r="E47">
         <v>34.77326636654423</v>
-      </c>
-      <c r="E47">
-        <v>6.872577378250044</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H47">
-        <v>6.872577378250044</v>
       </c>
     </row>
     <row r="48">
@@ -1802,18 +1281,7 @@
         <v>16.537385182788</v>
       </c>
       <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>5.231772101415717</v>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H48">
-        <v>-5.231772101415717</v>
+        <v>21.76915728420372</v>
       </c>
     </row>
     <row r="49">
@@ -1832,18 +1300,7 @@
         <v>32.46322064660833</v>
       </c>
       <c r="E49">
-        <v>0</v>
-      </c>
-      <c r="F49">
-        <v>21.30430452681811</v>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H49">
-        <v>-21.30430452681811</v>
+        <v>53.76752517342644</v>
       </c>
     </row>
     <row r="50">
@@ -1862,18 +1319,7 @@
         <v>20.59602260128642</v>
       </c>
       <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>9.674133984666955</v>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H50">
-        <v>-9.674133984666955</v>
+        <v>30.27015658595338</v>
       </c>
     </row>
     <row r="51">
@@ -1892,18 +1338,7 @@
         <v>20.78130542427902</v>
       </c>
       <c r="E51">
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <v>19.13467422617224</v>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H51">
-        <v>-19.13467422617224</v>
+        <v>39.91597965045125</v>
       </c>
     </row>
     <row r="52">
@@ -1922,18 +1357,7 @@
         <v>18.83320113624375</v>
       </c>
       <c r="E52">
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <v>12.56194598410228</v>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H52">
-        <v>-12.56194598410228</v>
+        <v>31.39514712034604</v>
       </c>
     </row>
     <row r="53">
@@ -1949,21 +1373,10 @@
         <v>51.31412260868171</v>
       </c>
       <c r="D53">
+        <v>51.3141226086817</v>
+      </c>
+      <c r="E53">
         <v>39.69989399621305</v>
-      </c>
-      <c r="E53">
-        <v>11.61422861246865</v>
-      </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H53">
-        <v>11.61422861246865</v>
       </c>
     </row>
     <row r="54">
@@ -1982,18 +1395,7 @@
         <v>21.1127970258937</v>
       </c>
       <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>15.71714253212478</v>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H54">
-        <v>-15.71714253212478</v>
+        <v>36.82993955801849</v>
       </c>
     </row>
     <row r="55">
@@ -2012,18 +1414,7 @@
         <v>35.5096309709038</v>
       </c>
       <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>0.9981771217672485</v>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H55">
-        <v>-0.9981771217672485</v>
+        <v>36.50780809267105</v>
       </c>
     </row>
     <row r="56">
@@ -2042,18 +1433,7 @@
         <v>19.11040153180073</v>
       </c>
       <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>22.23121626620409</v>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H56">
-        <v>-22.23121626620409</v>
+        <v>41.34161779800483</v>
       </c>
     </row>
     <row r="57">
@@ -2072,18 +1452,7 @@
         <v>26.95721536384507</v>
       </c>
       <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>25.41587075671615</v>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H57">
-        <v>-25.41587075671615</v>
+        <v>52.37308612056123</v>
       </c>
     </row>
     <row r="58">
@@ -2102,18 +1471,7 @@
         <v>31.48625875264324</v>
       </c>
       <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>15.40782253919257</v>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H58">
-        <v>-15.40782253919257</v>
+        <v>46.89408129183581</v>
       </c>
     </row>
     <row r="59">
@@ -2132,18 +1490,7 @@
         <v>30.97257244047038</v>
       </c>
       <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59">
-        <v>5.194711322094466</v>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H59">
-        <v>-5.194711322094466</v>
+        <v>36.16728376256484</v>
       </c>
     </row>
     <row r="60">
@@ -2162,18 +1509,7 @@
         <v>24.49183690477609</v>
       </c>
       <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>13.37411317735769</v>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H60">
-        <v>-13.37411317735769</v>
+        <v>37.86595008213377</v>
       </c>
     </row>
     <row r="61">
@@ -2192,18 +1528,7 @@
         <v>14.03189750987513</v>
       </c>
       <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>22.24429231423166</v>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H61">
-        <v>-22.24429231423166</v>
+        <v>36.27618982410679</v>
       </c>
     </row>
     <row r="62">
@@ -2222,18 +1547,7 @@
         <v>18.4566166970859</v>
       </c>
       <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62">
-        <v>19.35711391436251</v>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H62">
-        <v>-19.35711391436251</v>
+        <v>37.81373061144841</v>
       </c>
     </row>
     <row r="63">
@@ -2249,21 +1563,10 @@
         <v>54.75956598809968</v>
       </c>
       <c r="D63">
+        <v>54.75956598809966</v>
+      </c>
+      <c r="E63">
         <v>29.95244885123448</v>
-      </c>
-      <c r="E63">
-        <v>24.80711713686518</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H63">
-        <v>24.80711713686518</v>
       </c>
     </row>
     <row r="64">
@@ -2282,18 +1585,7 @@
         <v>30.83437827615269</v>
       </c>
       <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64">
-        <v>13.05178121008702</v>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H64">
-        <v>-13.05178121008702</v>
+        <v>43.88615948623971</v>
       </c>
     </row>
     <row r="65">
@@ -2312,18 +1604,7 @@
         <v>32.72278078191085</v>
       </c>
       <c r="E65">
-        <v>0</v>
-      </c>
-      <c r="F65">
-        <v>2.974217824469093</v>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H65">
-        <v>-2.974217824469093</v>
+        <v>35.69699860637994</v>
       </c>
     </row>
     <row r="66">
@@ -2342,18 +1623,7 @@
         <v>11.87907372922596</v>
       </c>
       <c r="E66">
-        <v>0</v>
-      </c>
-      <c r="F66">
-        <v>31.24432237727045</v>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H66">
-        <v>-31.24432237727045</v>
+        <v>43.12339610649641</v>
       </c>
     </row>
     <row r="67">
@@ -2369,21 +1639,10 @@
         <v>47.82142554126911</v>
       </c>
       <c r="D67">
+        <v>47.82142554126911</v>
+      </c>
+      <c r="E67">
         <v>37.12486576072786</v>
-      </c>
-      <c r="E67">
-        <v>10.69655978054125</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H67">
-        <v>10.69655978054125</v>
       </c>
     </row>
     <row r="68">
@@ -2402,18 +1661,7 @@
         <v>11.98786859245466</v>
       </c>
       <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
-        <v>6.139745349476067</v>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H68">
-        <v>-6.139745349476067</v>
+        <v>18.12761394193073</v>
       </c>
     </row>
     <row r="69">
@@ -2432,18 +1680,7 @@
         <v>10.8345354002511</v>
       </c>
       <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <v>53.96019916941266</v>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H69">
-        <v>-53.96019916941266</v>
+        <v>64.79473456966376</v>
       </c>
     </row>
     <row r="70">
@@ -2462,18 +1699,7 @@
         <v>16.95808325207584</v>
       </c>
       <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>28.96931626678109</v>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H70">
-        <v>-28.96931626678109</v>
+        <v>45.92739951885693</v>
       </c>
     </row>
     <row r="71">
@@ -2492,18 +1718,7 @@
         <v>34.26244252280595</v>
       </c>
       <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71">
-        <v>2.754947970499316</v>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H71">
-        <v>-2.754947970499316</v>
+        <v>37.01739049330526</v>
       </c>
     </row>
     <row r="72">
@@ -2522,18 +1737,7 @@
         <v>17.83014746805538</v>
       </c>
       <c r="E72">
-        <v>0</v>
-      </c>
-      <c r="F72">
-        <v>21.6518276609653</v>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H72">
-        <v>-21.6518276609653</v>
+        <v>39.48197512902068</v>
       </c>
     </row>
     <row r="73">
@@ -2552,18 +1756,7 @@
         <v>13.74649178074346</v>
       </c>
       <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="F73">
-        <v>22.83290970802051</v>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H73">
-        <v>-22.83290970802051</v>
+        <v>36.57940148876396</v>
       </c>
     </row>
     <row r="74">
@@ -2582,18 +1775,7 @@
         <v>28.15331827912842</v>
       </c>
       <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74">
-        <v>11.97967553082801</v>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H74">
-        <v>-11.97967553082801</v>
+        <v>40.13299380995643</v>
       </c>
     </row>
     <row r="75">
@@ -2612,18 +1794,7 @@
         <v>8.622068442841503</v>
       </c>
       <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75">
-        <v>30.61087557521233</v>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H75">
-        <v>-30.61087557521233</v>
+        <v>39.23294401805384</v>
       </c>
     </row>
     <row r="76">
@@ -2642,18 +1813,7 @@
         <v>23.20003292907899</v>
       </c>
       <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76">
-        <v>14.19770857766031</v>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H76">
-        <v>-14.19770857766031</v>
+        <v>37.39774150673931</v>
       </c>
     </row>
     <row r="77">
@@ -2672,18 +1832,7 @@
         <v>25.15406867060747</v>
       </c>
       <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <v>5.377183359442459</v>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H77">
-        <v>-5.377183359442459</v>
+        <v>30.53125203004993</v>
       </c>
     </row>
     <row r="78">
@@ -2699,21 +1848,10 @@
         <v>34.19031354227034</v>
       </c>
       <c r="D78">
+        <v>34.19031354227033</v>
+      </c>
+      <c r="E78">
         <v>31.46269485028784</v>
-      </c>
-      <c r="E78">
-        <v>2.727618691982488</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H78">
-        <v>2.727618691982488</v>
       </c>
     </row>
     <row r="79">
@@ -2729,21 +1867,10 @@
         <v>31.79118989550677</v>
       </c>
       <c r="D79">
+        <v>31.79118989550678</v>
+      </c>
+      <c r="E79">
         <v>20.84422268367878</v>
-      </c>
-      <c r="E79">
-        <v>10.94696721182799</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H79">
-        <v>10.94696721182799</v>
       </c>
     </row>
     <row r="80">
@@ -2762,18 +1889,7 @@
         <v>31.92564871144535</v>
       </c>
       <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
-        <v>5.8978356739928</v>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H80">
-        <v>-5.8978356739928</v>
+        <v>37.82348438543815</v>
       </c>
     </row>
     <row r="81">
@@ -2789,21 +1905,10 @@
         <v>34.10371916957992</v>
       </c>
       <c r="D81">
+        <v>34.10371916957991</v>
+      </c>
+      <c r="E81">
         <v>23.94870609522823</v>
-      </c>
-      <c r="E81">
-        <v>10.15501307435168</v>
-      </c>
-      <c r="F81">
-        <v>0</v>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H81">
-        <v>10.15501307435168</v>
       </c>
     </row>
     <row r="82">
@@ -2819,21 +1924,10 @@
         <v>51.97583239295577</v>
       </c>
       <c r="D82">
+        <v>51.97583239295577</v>
+      </c>
+      <c r="E82">
         <v>27.98096525845754</v>
-      </c>
-      <c r="E82">
-        <v>23.99486713449823</v>
-      </c>
-      <c r="F82">
-        <v>0</v>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H82">
-        <v>23.99486713449823</v>
       </c>
     </row>
     <row r="83">
@@ -2852,18 +1946,7 @@
         <v>27.91245198754862</v>
       </c>
       <c r="E83">
-        <v>0</v>
-      </c>
-      <c r="F83">
-        <v>5.482024333939871</v>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H83">
-        <v>-5.482024333939871</v>
+        <v>33.39447632148849</v>
       </c>
     </row>
     <row r="84">
@@ -2879,21 +1962,10 @@
         <v>38.59750695193733</v>
       </c>
       <c r="D84">
+        <v>38.59750695193734</v>
+      </c>
+      <c r="E84">
         <v>30.80185770807167</v>
-      </c>
-      <c r="E84">
-        <v>7.795649243865667</v>
-      </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H84">
-        <v>7.795649243865667</v>
       </c>
     </row>
     <row r="85">
@@ -2909,21 +1981,10 @@
         <v>35.47144548638347</v>
       </c>
       <c r="D85">
+        <v>35.47144548638347</v>
+      </c>
+      <c r="E85">
         <v>27.54284935920796</v>
-      </c>
-      <c r="E85">
-        <v>7.928596127175509</v>
-      </c>
-      <c r="F85">
-        <v>0</v>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H85">
-        <v>7.928596127175509</v>
       </c>
     </row>
     <row r="86">
@@ -2942,18 +2003,7 @@
         <v>26.88384331424021</v>
       </c>
       <c r="E86">
-        <v>0</v>
-      </c>
-      <c r="F86">
-        <v>2.124602644173061</v>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H86">
-        <v>-2.124602644173061</v>
+        <v>29.00844595841327</v>
       </c>
     </row>
     <row r="87">
@@ -2969,21 +2019,10 @@
         <v>36.33942303684283</v>
       </c>
       <c r="D87">
+        <v>36.33942303684284</v>
+      </c>
+      <c r="E87">
         <v>36.28217008326812</v>
-      </c>
-      <c r="E87">
-        <v>0.05725295357471848</v>
-      </c>
-      <c r="F87">
-        <v>0</v>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H87">
-        <v>0.05725295357471848</v>
       </c>
     </row>
     <row r="88">
@@ -3002,18 +2041,7 @@
         <v>25.89276081562196</v>
       </c>
       <c r="E88">
-        <v>0</v>
-      </c>
-      <c r="F88">
-        <v>6.253776964232176</v>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H88">
-        <v>-6.253776964232176</v>
+        <v>32.14653777985414</v>
       </c>
     </row>
     <row r="89">
@@ -3032,18 +2060,7 @@
         <v>17.76461880088823</v>
       </c>
       <c r="E89">
-        <v>0</v>
-      </c>
-      <c r="F89">
-        <v>31.4560993053047</v>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H89">
-        <v>-31.4560993053047</v>
+        <v>49.22071810619293</v>
       </c>
     </row>
     <row r="90">
@@ -3062,18 +2079,7 @@
         <v>26.29848783694937</v>
       </c>
       <c r="E90">
-        <v>0</v>
-      </c>
-      <c r="F90">
-        <v>12.29176071117761</v>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H90">
-        <v>-12.29176071117761</v>
+        <v>38.59024854812698</v>
       </c>
     </row>
     <row r="91">
@@ -3092,18 +2098,7 @@
         <v>15.11474723248645</v>
       </c>
       <c r="E91">
-        <v>0</v>
-      </c>
-      <c r="F91">
-        <v>23.72497076334519</v>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H91">
-        <v>-23.72497076334519</v>
+        <v>38.83971799583164</v>
       </c>
     </row>
     <row r="92">
@@ -3122,18 +2117,7 @@
         <v>31.47552777715326</v>
       </c>
       <c r="E92">
-        <v>0</v>
-      </c>
-      <c r="F92">
-        <v>11.17347825787446</v>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H92">
-        <v>-11.17347825787446</v>
+        <v>42.64900603502772</v>
       </c>
     </row>
     <row r="93">
@@ -3152,18 +2136,7 @@
         <v>10.77850834510538</v>
       </c>
       <c r="E93">
-        <v>0</v>
-      </c>
-      <c r="F93">
-        <v>38.21705192467589</v>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H93">
-        <v>-38.21705192467589</v>
+        <v>48.99556026978128</v>
       </c>
     </row>
     <row r="94">
@@ -3182,18 +2155,7 @@
         <v>20.87569682302821</v>
       </c>
       <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="F94">
-        <v>22.98559178115814</v>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H94">
-        <v>-22.98559178115814</v>
+        <v>43.86128860418636</v>
       </c>
     </row>
     <row r="95">
@@ -3209,21 +2171,10 @@
         <v>42.58449150245828</v>
       </c>
       <c r="D95">
+        <v>42.58449150245828</v>
+      </c>
+      <c r="E95">
         <v>37.90085510855813</v>
-      </c>
-      <c r="E95">
-        <v>4.683636393900156</v>
-      </c>
-      <c r="F95">
-        <v>0</v>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H95">
-        <v>4.683636393900156</v>
       </c>
     </row>
     <row r="96">
@@ -3242,18 +2193,7 @@
         <v>9.523476068765097</v>
       </c>
       <c r="E96">
-        <v>0</v>
-      </c>
-      <c r="F96">
-        <v>44.05713182774148</v>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H96">
-        <v>-44.05713182774148</v>
+        <v>53.58060789650658</v>
       </c>
     </row>
     <row r="97">
@@ -3269,21 +2209,10 @@
         <v>31.98827013782962</v>
       </c>
       <c r="D97">
+        <v>31.98827013782961</v>
+      </c>
+      <c r="E97">
         <v>26.67571174349406</v>
-      </c>
-      <c r="E97">
-        <v>5.312558394335558</v>
-      </c>
-      <c r="F97">
-        <v>0</v>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H97">
-        <v>5.312558394335558</v>
       </c>
     </row>
     <row r="98">
@@ -3302,18 +2231,7 @@
         <v>26.51396420839526</v>
       </c>
       <c r="E98">
-        <v>0</v>
-      </c>
-      <c r="F98">
-        <v>1.1315602680516</v>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H98">
-        <v>-1.1315602680516</v>
+        <v>27.64552447644686</v>
       </c>
     </row>
     <row r="99">
@@ -3332,18 +2250,7 @@
         <v>34.3832504451403</v>
       </c>
       <c r="E99">
-        <v>0</v>
-      </c>
-      <c r="F99">
-        <v>2.276079272338747</v>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H99">
-        <v>-2.276079272338747</v>
+        <v>36.65932971747905</v>
       </c>
     </row>
     <row r="100">
@@ -3362,18 +2269,7 @@
         <v>22.50289469054428</v>
       </c>
       <c r="E100">
-        <v>0</v>
-      </c>
-      <c r="F100">
-        <v>8.200958229735916</v>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H100">
-        <v>-8.200958229735916</v>
+        <v>30.7038529202802</v>
       </c>
     </row>
     <row r="101">
@@ -3392,18 +2288,7 @@
         <v>25.98752598752599</v>
       </c>
       <c r="E101">
-        <v>0</v>
-      </c>
-      <c r="F101">
-        <v>13.78444243729935</v>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>S6</t>
-        </is>
-      </c>
-      <c r="H101">
-        <v>-13.78444243729935</v>
+        <v>39.77196842482534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>